<commit_message>
Added main class. Code refactoring and comments.
</commit_message>
<xml_diff>
--- a/intrastat/intrastat_test/Intrastat Submission Sample.xlsx
+++ b/intrastat/intrastat_test/Intrastat Submission Sample.xlsx
@@ -489,10 +489,8 @@
       <c r="C2" t="n">
         <v>2121.407</v>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="D2" t="n">
+        <v>1</v>
       </c>
       <c r="E2" t="n">
         <v>0.595</v>
@@ -527,10 +525,8 @@
       <c r="C3" t="n">
         <v>1668.27</v>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="D3" t="n">
+        <v>1</v>
       </c>
       <c r="E3" t="n">
         <v>0.678</v>
@@ -565,10 +561,8 @@
       <c r="C4" t="n">
         <v>1957.34</v>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="D4" t="n">
+        <v>1</v>
       </c>
       <c r="E4" t="n">
         <v>0.704</v>
@@ -603,10 +597,8 @@
       <c r="C5" t="n">
         <v>1519.83</v>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="D5" t="n">
+        <v>1</v>
       </c>
       <c r="E5" t="n">
         <v>0.844</v>
@@ -641,10 +633,8 @@
       <c r="C6" t="n">
         <v>1619.1135</v>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="D6" t="n">
+        <v>1</v>
       </c>
       <c r="E6" t="n">
         <v>0.461</v>
@@ -679,10 +669,8 @@
       <c r="C7" t="n">
         <v>1782.88</v>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="D7" t="n">
+        <v>1</v>
       </c>
       <c r="E7" t="n">
         <v>0.589</v>
@@ -717,10 +705,8 @@
       <c r="C8" t="n">
         <v>1733.644</v>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="D8" t="n">
+        <v>1</v>
       </c>
       <c r="E8" t="n">
         <v>0.533</v>
@@ -755,10 +741,8 @@
       <c r="C9" t="n">
         <v>2026.44</v>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="D9" t="n">
+        <v>1</v>
       </c>
       <c r="E9" t="n">
         <v>0.406</v>

</xml_diff>